<commit_message>
feat: Remove internal round and float casts
This patch removes any internal rounding of floating point values
throughout the simulation. At various locations floating point values
are restricted to a small number of decimal places, e.g. using
`round(..., 4)`, or explicitly cast to integer values through
`round(...)` and `int(...)`.

Small changes in floating point values can change the way these values
are truncated, rounded, or cast to integers, resulting in relatively
large numerical differences in reference output of subsequent files.

By removing all intermediate rounding, the reference files need to be
updated to reflect the changes in resulting values.
</commit_message>
<xml_diff>
--- a/tests/vlaanderen/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
+++ b/tests/vlaanderen/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
@@ -388,16 +388,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>516</v>
+        <v>519.5399500817239</v>
       </c>
       <c r="C2">
-        <v>978</v>
+        <v>981.181658104533</v>
       </c>
       <c r="D2">
-        <v>1324</v>
+        <v>1329.718121219282</v>
       </c>
       <c r="E2">
-        <v>1480</v>
+        <v>1482.659367292297</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -405,16 +405,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>539</v>
+        <v>542.3516677527452</v>
       </c>
       <c r="C3">
-        <v>996</v>
+        <v>1001.504143663945</v>
       </c>
       <c r="D3">
-        <v>1336</v>
+        <v>1340.620711963814</v>
       </c>
       <c r="E3">
-        <v>1483</v>
+        <v>1489.660156732298</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -422,16 +422,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>563</v>
+        <v>563.8605507489592</v>
       </c>
       <c r="C4">
-        <v>1038</v>
+        <v>1039.496240544647</v>
       </c>
       <c r="D4">
-        <v>1381</v>
+        <v>1385.142876463339</v>
       </c>
       <c r="E4">
-        <v>1533</v>
+        <v>1536.745462111212</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -439,16 +439,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>661</v>
+        <v>662.9786698217429</v>
       </c>
       <c r="C5">
-        <v>1126</v>
+        <v>1131.549665732404</v>
       </c>
       <c r="D5">
-        <v>1432</v>
+        <v>1436.697173459555</v>
       </c>
       <c r="E5">
-        <v>1585</v>
+        <v>1589.172341735097</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -456,16 +456,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>645</v>
+        <v>647.8814483192817</v>
       </c>
       <c r="C6">
-        <v>1119</v>
+        <v>1122.600416929733</v>
       </c>
       <c r="D6">
-        <v>1428</v>
+        <v>1432.230304965013</v>
       </c>
       <c r="E6">
-        <v>1583</v>
+        <v>1586.12702903763</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -473,16 +473,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>712</v>
+        <v>713.9659208237927</v>
       </c>
       <c r="C7">
-        <v>1173</v>
+        <v>1176.796944956915</v>
       </c>
       <c r="D7">
-        <v>1470</v>
+        <v>1471.982866696806</v>
       </c>
       <c r="E7">
-        <v>1590</v>
+        <v>1595.448448823696</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -490,16 +490,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>286</v>
+        <v>285.6775235257514</v>
       </c>
       <c r="C8">
-        <v>723</v>
+        <v>722.3126791818364</v>
       </c>
       <c r="D8">
-        <v>1117</v>
+        <v>1114.811042334584</v>
       </c>
       <c r="E8">
-        <v>1432</v>
+        <v>1433.203986887945</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -507,16 +507,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>605</v>
+        <v>606.6176074155284</v>
       </c>
       <c r="C9">
-        <v>1061</v>
+        <v>1065.463844133058</v>
       </c>
       <c r="D9">
-        <v>1390</v>
+        <v>1396.439384704664</v>
       </c>
       <c r="E9">
-        <v>1539</v>
+        <v>1546.589363101275</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -524,16 +524,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>681</v>
+        <v>683.4259752372587</v>
       </c>
       <c r="C10">
-        <v>1154</v>
+        <v>1157.648520803099</v>
       </c>
       <c r="D10">
-        <v>1461</v>
+        <v>1464.053630130737</v>
       </c>
       <c r="E10">
-        <v>1587</v>
+        <v>1589.572658536279</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -541,16 +541,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>683</v>
+        <v>686.6652809504774</v>
       </c>
       <c r="C11">
-        <v>1156</v>
+        <v>1160.705684869071</v>
       </c>
       <c r="D11">
-        <v>1462</v>
+        <v>1466.482912877761</v>
       </c>
       <c r="E11">
-        <v>1589</v>
+        <v>1591.98943187592</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -558,16 +558,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>700</v>
+        <v>700.8260013260174</v>
       </c>
       <c r="C12">
-        <v>1169</v>
+        <v>1172.403438093525</v>
       </c>
       <c r="D12">
-        <v>1467</v>
+        <v>1471.719828093797</v>
       </c>
       <c r="E12">
-        <v>1591</v>
+        <v>1594.044308298733</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -575,16 +575,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>680</v>
+        <v>681.6785216095993</v>
       </c>
       <c r="C13">
-        <v>1152</v>
+        <v>1155.606495902057</v>
       </c>
       <c r="D13">
-        <v>1459</v>
+        <v>1462.307684232907</v>
       </c>
       <c r="E13">
-        <v>1584</v>
+        <v>1587.962461674932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: Update references to integer format
The `Ontpl_` and `Pot_` files only need to be written to disk as integer
data. This is now reflected in the test references for test cases
`eindhoven-500` and `vlaanderen`.
</commit_message>
<xml_diff>
--- a/tests/vlaanderen/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
+++ b/tests/vlaanderen/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
@@ -388,16 +388,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>519.539950081724</v>
+        <v>520</v>
       </c>
       <c r="C2">
-        <v>981.1816581045335</v>
+        <v>981</v>
       </c>
       <c r="D2">
-        <v>1329.718121219282</v>
+        <v>1330</v>
       </c>
       <c r="E2">
-        <v>1482.659367292297</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -405,16 +405,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>542.351667752745</v>
+        <v>542</v>
       </c>
       <c r="C3">
-        <v>1001.504143663945</v>
+        <v>1002</v>
       </c>
       <c r="D3">
-        <v>1340.620711963814</v>
+        <v>1341</v>
       </c>
       <c r="E3">
-        <v>1489.660156732299</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -422,16 +422,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>563.8605507489586</v>
+        <v>564</v>
       </c>
       <c r="C4">
-        <v>1039.496240544647</v>
+        <v>1039</v>
       </c>
       <c r="D4">
-        <v>1385.142876463339</v>
+        <v>1385</v>
       </c>
       <c r="E4">
-        <v>1536.745462111212</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -439,16 +439,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>662.9786698217432</v>
+        <v>663</v>
       </c>
       <c r="C5">
-        <v>1131.549665732404</v>
+        <v>1132</v>
       </c>
       <c r="D5">
-        <v>1436.697173459556</v>
+        <v>1437</v>
       </c>
       <c r="E5">
-        <v>1589.172341735097</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -456,16 +456,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>647.8814483192821</v>
+        <v>648</v>
       </c>
       <c r="C6">
-        <v>1122.600416929733</v>
+        <v>1123</v>
       </c>
       <c r="D6">
-        <v>1432.230304965012</v>
+        <v>1432</v>
       </c>
       <c r="E6">
-        <v>1586.127029037631</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -473,16 +473,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>713.9659208237925</v>
+        <v>714</v>
       </c>
       <c r="C7">
-        <v>1176.796944956915</v>
+        <v>1177</v>
       </c>
       <c r="D7">
-        <v>1471.982866696805</v>
+        <v>1472</v>
       </c>
       <c r="E7">
-        <v>1595.448448823695</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -490,16 +490,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>285.6775235257509</v>
+        <v>286</v>
       </c>
       <c r="C8">
-        <v>722.3126791818363</v>
+        <v>722</v>
       </c>
       <c r="D8">
-        <v>1114.811042334585</v>
+        <v>1115</v>
       </c>
       <c r="E8">
-        <v>1433.203986887945</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -507,16 +507,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>606.6176074155286</v>
+        <v>607</v>
       </c>
       <c r="C9">
-        <v>1065.463844133058</v>
+        <v>1065</v>
       </c>
       <c r="D9">
-        <v>1396.439384704664</v>
+        <v>1396</v>
       </c>
       <c r="E9">
-        <v>1546.589363101276</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -524,16 +524,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>683.4259752372591</v>
+        <v>683</v>
       </c>
       <c r="C10">
-        <v>1157.648520803098</v>
+        <v>1158</v>
       </c>
       <c r="D10">
-        <v>1464.053630130737</v>
+        <v>1464</v>
       </c>
       <c r="E10">
-        <v>1589.572658536279</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -541,16 +541,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>686.6652809504775</v>
+        <v>687</v>
       </c>
       <c r="C11">
-        <v>1160.705684869072</v>
+        <v>1161</v>
       </c>
       <c r="D11">
-        <v>1466.482912877761</v>
+        <v>1466</v>
       </c>
       <c r="E11">
-        <v>1591.98943187592</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -558,16 +558,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>700.826001326017</v>
+        <v>701</v>
       </c>
       <c r="C12">
-        <v>1172.403438093525</v>
+        <v>1172</v>
       </c>
       <c r="D12">
-        <v>1471.719828093798</v>
+        <v>1472</v>
       </c>
       <c r="E12">
-        <v>1594.044308298733</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -575,16 +575,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>681.6785216095994</v>
+        <v>682</v>
       </c>
       <c r="C13">
-        <v>1155.606495902056</v>
+        <v>1156</v>
       </c>
       <c r="D13">
-        <v>1462.307684232907</v>
+        <v>1462</v>
       </c>
       <c r="E13">
-        <v>1587.962461674932</v>
+        <v>1588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>